<commit_message>
fc with final power report
</commit_message>
<xml_diff>
--- a/hw_model/fully_connected_4x4/verify outputs.xlsx
+++ b/hw_model/fully_connected_4x4/verify outputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Desktop\Workshop\Componenti\fully_connected_4x4_unif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Desktop\fully_connected_4x4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1872993D-B541-4EBE-AE04-69119D8FA14F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8455DED6-08A7-4ABE-AA25-7D7F50C06997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>